<commit_message>
Assessment 2 -Task 2 Code Changes.
Assessment 2 -Task 2 Code Changes.
</commit_message>
<xml_diff>
--- a/Product Backlog/AK_Product-backlog-template.xlsx
+++ b/Product Backlog/AK_Product-backlog-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apurvakedar/Downloads/snakegame_v1/Product Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B47D188-0AD5-1645-A00D-205F7944E113}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754EC432-0546-0142-AF73-38C91FE684BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{49C32462-D2B8-4175-AE19-832EFB3F644D}"/>
   </bookViews>
@@ -136,13 +136,6 @@
     <t>Apurva Kedar 23796845</t>
   </si>
   <si>
-    <t> the game board looks like :
-a) the background color is black
-b) the snake color is green
-c) the apple color is red
-d) the default board size is 400px by 400px</t>
-  </si>
-  <si>
     <t>Show the snake. The snake head looks like a pre loaded image and snake can move in upward, downward, left, right directions based on user inputs of respective arrow keys</t>
   </si>
   <si>
@@ -153,6 +146,13 @@
   </si>
   <si>
     <t>The game is over if Snake Body hits the boundaries of the board and a message is displayed to the player.</t>
+  </si>
+  <si>
+    <t> The game board looks like :
+a) The background color is black
+b) The snake color is green
+c) The apple color is red
+d) The default board size is 400px by 400px</t>
   </si>
 </sst>
 </file>
@@ -650,7 +650,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -738,7 +738,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -746,7 +746,7 @@
         <v>3</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -754,7 +754,7 @@
         <v>4</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -762,7 +762,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -770,7 +770,7 @@
         <v>6</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>